<commit_message>
Add correct option handling to question import: update model, migration, and view
</commit_message>
<xml_diff>
--- a/public/uploads/Question-format.xlsx
+++ b/public/uploads/Question-format.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28021"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\navy-exam\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\navy-question\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49B49D4-EBDA-4C5A-B6C3-52954F753641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="1440" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4524" yWindow="1440" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>option_1</t>
   </si>
@@ -43,12 +42,15 @@
   </si>
   <si>
     <t>mark</t>
+  </si>
+  <si>
+    <t>correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,11 +361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,7 +373,7 @@
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -389,6 +391,9 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>